<commit_message>
fixes for UI and new features
</commit_message>
<xml_diff>
--- a/excel/data0.xlsx
+++ b/excel/data0.xlsx
@@ -442,7 +442,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>04/15/2025 09:08:05 PM</t>
+          <t>04/17/2025 02:53:14 PM</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -458,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,7 +469,7 @@
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="13" customWidth="1" min="3" max="3"/>
-    <col width="33" customWidth="1" min="4" max="4"/>
+    <col width="36" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
@@ -538,13 +538,13 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4-6mm model</t>
+          <t>2-4mm model</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>03.Sample3_ST4_4-6mm_8-6-24.JPG</t>
+          <t>01.Sample1_ST3_2-4mm_6-12-24_1.jpeg</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -558,169 +558,9 @@
         <v/>
       </c>
       <c r="I3" t="n">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="J3" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>4-6mm model</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>03.Sample3_ST4_4-6mm_8-6-24.JPG</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v/>
-      </c>
-      <c r="G4" t="n">
-        <v/>
-      </c>
-      <c r="H4" t="n">
-        <v/>
-      </c>
-      <c r="I4" t="n">
-        <v>41</v>
-      </c>
-      <c r="J4" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4-6mm model</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>03.Sample3_ST4_4-6mm_8-6-24.JPG</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v/>
-      </c>
-      <c r="G5" t="n">
-        <v/>
-      </c>
-      <c r="H5" t="n">
-        <v/>
-      </c>
-      <c r="I5" t="n">
-        <v>41</v>
-      </c>
-      <c r="J5" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4-6mm model</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>03.Sample3_ST4_4-6mm_8-6-24.JPG</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v/>
-      </c>
-      <c r="G6" t="n">
-        <v/>
-      </c>
-      <c r="H6" t="n">
-        <v/>
-      </c>
-      <c r="I6" t="n">
-        <v>41</v>
-      </c>
-      <c r="J6" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>4-6mm model</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>03.Sample3_ST4_4-6mm_8-6-24.JPG</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v/>
-      </c>
-      <c r="G7" t="n">
-        <v/>
-      </c>
-      <c r="H7" t="n">
-        <v/>
-      </c>
-      <c r="I7" t="n">
-        <v>41</v>
-      </c>
-      <c r="J7" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>4-6mm model</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>01.Sample1_ST4_4-6mm_7-30-24.JPG</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v/>
-      </c>
-      <c r="G8" t="n">
-        <v/>
-      </c>
-      <c r="H8" t="n">
-        <v/>
-      </c>
-      <c r="I8" t="n">
-        <v>45</v>
-      </c>
-      <c r="J8" t="n">
         <v/>
       </c>
     </row>
@@ -797,7 +637,7 @@
         <v/>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v/>

</xml_diff>